<commit_message>
Third draft and launch attempt
</commit_message>
<xml_diff>
--- a/data/hh3_data.xlsx
+++ b/data/hh3_data.xlsx
@@ -17,8 +17,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">army_lists!$A$1:$G$108</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">hero_constraints!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">keywords!$A$1:$D$49</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">models!$A$1:$P$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">keywords!$A$1:$D$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">models!$A$1:$P$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">options!$A$1:$I$1387</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">warning_rules!$A$1:$D$1</definedName>
   </definedNames>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="350">
   <si>
     <t>model_id</t>
   </si>
@@ -240,24 +240,6 @@
     <t>Iron Warriors</t>
   </si>
   <si>
-    <t>Legion Praetor</t>
-  </si>
-  <si>
-    <t>Legion Cataphractii Praetor</t>
-  </si>
-  <si>
-    <t>Legion Tartaros Praetor</t>
-  </si>
-  <si>
-    <t>Legion Centurion</t>
-  </si>
-  <si>
-    <t>Legion Cataphractii Centurion</t>
-  </si>
-  <si>
-    <t>Legion Tartaros Centurion</t>
-  </si>
-  <si>
     <t>Legion Command Squad</t>
   </si>
   <si>
@@ -273,12 +255,6 @@
     <t>Legion Veteran Squad</t>
   </si>
   <si>
-    <t>Legion Terminator Cataphractii Squad</t>
-  </si>
-  <si>
-    <t>Legion Terminator Tartaros Squad</t>
-  </si>
-  <si>
     <t>High Command</t>
   </si>
   <si>
@@ -318,9 +294,6 @@
     <t>Legion Contemptor Dreadnought</t>
   </si>
   <si>
-    <t>Legion Tactical Squad</t>
-  </si>
-  <si>
     <t>Troops</t>
   </si>
   <si>
@@ -363,9 +336,6 @@
     <t>Legion Dreadnought Drop Pod</t>
   </si>
   <si>
-    <t>Exchange both his bolt pistol and chainsword for two lightning claws</t>
-  </si>
-  <si>
     <t>Bolter</t>
   </si>
   <si>
@@ -454,13 +424,6 @@
   </si>
   <si>
     <t>Legiones Astartes (Iron Warrior)</t>
-  </si>
-  <si>
-    <t>A Detachment selected from this Army List is considered to be of the Legiones Astartes (Iron Warrior).
-Note that all units selected as part of a given Detachment must have the Legiones Astartes (Iron Warrior) special rule, or no variant of that special rule.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The greatest commanders of the Space Marine Legions are all  but peerless in their strategic and tactical abilities. The gene craft of the Emperor that created them, honed by individual talent and the experience of countless battles, has sharpened their acumen to a preternatural degree.</t>
   </si>
   <si>
     <t>Astartes</t>
@@ -477,18 +440,6 @@
 ]</t>
   </si>
   <si>
-    <t>[
-    {
-        "title": "\"Wrack &amp; Ruin"\",
-        "description": "When a model with this special rule makes a Shooting Attack or Melee Attack targeting a model with the Dreadnought, Automata, Vehicle or Building Unit Type, it gains +1 to the Strength of that attack."
-    },
-    {
-        "title": "Warsmiths",
-        "description": " A Detachment with this special rule may choose to upgrade a Legion Praetor, Legion Cataphractii Praetor or Legion Tartaros Praetor to a Warsmith (see The Armoury of the Iron Warriors section for details)."
-    }
-]</t>
-  </si>
-  <si>
     <t>[astartes] legion-praetor</t>
   </si>
   <si>
@@ -582,20 +533,10 @@
     <t>[astartes] legion-termite-assault-drill</t>
   </si>
   <si>
-    <t>Legiones Astartes (X)</t>
-  </si>
-  <si>
-    <t>A Detachment selected from this Army List is considered to be of a specific Legion.
-Note that all units selected as part of a given Detachment must have the Legiones Astartes (X) special rule, or no variant of that special rule.</t>
-  </si>
-  <si>
     <t>[astartes] crusade-primary-detachment</t>
   </si>
   <si>
     <t>[astartes] shock-assault</t>
-  </si>
-  <si>
-    <t>['[astartes] legion-terminator-cataphractii-squad', '[astartes] legion-terminator-tartaros-squad']</t>
   </si>
   <si>
     <t>[astartes] army-vanguard</t>
@@ -703,32 +644,488 @@
     <t>This army's primary detachment is the Crusade Primary Detachment and must be selected.</t>
   </si>
   <si>
-    <t>Legiones Astartes [Apex]</t>
-  </si>
-  <si>
-    <t>Legiones Astartes [Auxillary]</t>
-  </si>
-  <si>
-    <t>['[astartes] legion-praetor', '[astartes] legion-cataphractii-praetor', '[astartes] legion-tartaros-praetor', '[astartes] legion-centurion', '[astartes] legion-cataphractii-centurion', '[astartes] legion-tartaros-centurion', '[astartes] legion-damocles-command-rhino', '[astartes] legion-tactical-squad', '[astartes] legion-despoiler-squad', '[astartes] legion-assault-squad', '[astartes] legion-breacher-squad', '[astartes] legion-rhino', '[astartes] legion-drop-pod', '[astartes] legion-termite-assault-drill']</t>
-  </si>
-  <si>
-    <t>["[astartes] legion-praetor", "[astartes] legion-cataphractii-praetor", "[astartes] legion-tartaros-praetor"]</t>
-  </si>
-  <si>
-    <t>A High Command is required to select an Apex Detachment.</t>
-  </si>
-  <si>
     <t>["[astartes] legion-centurion", "[astartes] legion-cataphractii-centurion", "[astartes] legion-tartaros-centurion", "[astartes] legion-damocles-command-rhino"]</t>
   </si>
   <si>
     <t>A Command sub-type model is required to select an Auxillary Detachment.</t>
+  </si>
+  <si>
+    <t>mount</t>
+  </si>
+  <si>
+    <t>Primarch</t>
+  </si>
+  <si>
+    <t>Perturabo</t>
+  </si>
+  <si>
+    <t>Warlord</t>
+  </si>
+  <si>
+    <t>[iron-warriors] warlord-perturabo</t>
+  </si>
+  <si>
+    <t>[astartes] legion-fellblade</t>
+  </si>
+  <si>
+    <t>Legion Fellblade</t>
+  </si>
+  <si>
+    <t>Lord of War</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "title": "\"Wrack &amp; Ruin\"",
+        "description": "When a model with this special rule makes a Shooting Attack or Melee Attack targeting a model with the Dreadnought, Automata, Vehicle or Building Unit Type, it gains +1 to the Strength of that attack."
+    },
+    {
+        "title": "Warsmiths",
+        "description": " A Detachment with this special rule may choose to upgrade a Legion Praetor, Legion Cataphractii Praetor or Legion Tartaros Praetor to a Warsmith (see The Armoury of the Iron Warriors section for details)."
+    }
+]</t>
+  </si>
+  <si>
+    <t>A Detachment selected from this Army List is considered to be of a specific Legion. Note that all units selected as part of a given Detachment must have the Legiones Astartes (X) special rule, or no variant of that special rule.</t>
+  </si>
+  <si>
+    <t>['[astartes] legion-command-squad', '[astartes] legion-cataphractii-command-squad', '[astartes] legion-tartaros-command-squad']</t>
+  </si>
+  <si>
+    <t>A Detachment selected from this Army List is considered to be of the Legiones Astartes (Iron Warrior). Note that all units selected as part of a given Detachment must have the Legiones Astartes (Iron Warrior) special rule, or no variant of that special rule.</t>
+  </si>
+  <si>
+    <t>May select a rite of war. May select one Apex Detachment.</t>
+  </si>
+  <si>
+    <t>Apex Detachment</t>
+  </si>
+  <si>
+    <t>Auxillary Detachment</t>
+  </si>
+  <si>
+    <t>A Master of the Legion is required to select an Apex Detachment.</t>
+  </si>
+  <si>
+    <t>Bulky (X)</t>
+  </si>
+  <si>
+    <t>Explodes (X)</t>
+  </si>
+  <si>
+    <t>Implacable Advance</t>
+  </si>
+  <si>
+    <t>Slow and Purposeful</t>
+  </si>
+  <si>
+    <t>[Legiones Astartes]</t>
+  </si>
+  <si>
+    <t>[Allegiance]</t>
+  </si>
+  <si>
+    <t>Barrage (X)</t>
+  </si>
+  <si>
+    <t>Blast (X)</t>
+  </si>
+  <si>
+    <t>Breaching (X)</t>
+  </si>
+  <si>
+    <t>Overload (X)</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>Reaping Blow (X)</t>
+  </si>
+  <si>
+    <t>Critical Hit (X)</t>
+  </si>
+  <si>
+    <t>Suppressive (X)</t>
+  </si>
+  <si>
+    <t>Fear (X)</t>
+  </si>
+  <si>
+    <t>Fast (X)</t>
+  </si>
+  <si>
+    <t>Feel No Pain (X)</t>
+  </si>
+  <si>
+    <t>Shread (X)</t>
+  </si>
+  <si>
+    <t>Rending (X)</t>
+  </si>
+  <si>
+    <t>Deep Strike</t>
+  </si>
+  <si>
+    <t>Firing Protocols (X)</t>
+  </si>
+  <si>
+    <t>Hatred (X)</t>
+  </si>
+  <si>
+    <t>Force (X)</t>
+  </si>
+  <si>
+    <t>Heavy (X)</t>
+  </si>
+  <si>
+    <t>Vanguard (X)</t>
+  </si>
+  <si>
+    <t>Weapons and other attacks that have the Suppressive (X) Special Rule have a chance of inflicting the Suppressed Status on the Target Unit.</t>
+  </si>
+  <si>
+    <t>Weapons and attacks with the Template Special Rule use the Flame Template to determine how many Models they Hit.</t>
+  </si>
+  <si>
+    <t>A Unit that includes Models with this Special Rule scores fewer Victory Points for controlling Objectives, but can score Victory Points for destroying enemy Units that hold Objectives.</t>
+  </si>
+  <si>
+    <t>If a Model with this Special Rule is outnumbered, it gains extra attacks.</t>
+  </si>
+  <si>
+    <t>With a Weapon that has the Rending (X) Special Rule, there is a chance that a Hit Test may result in an automatic wound.</t>
+  </si>
+  <si>
+    <t>Shock (X)</t>
+  </si>
+  <si>
+    <t>Shrouded (X)</t>
+  </si>
+  <si>
+    <t>Weapons with the Shock (X) Special Rule have a chance of inflicting Statuses on Vehicles even if it does not penetrate their armour.</t>
+  </si>
+  <si>
+    <t>Attacks made with the Shread (X) Special Rule can sometimes inflict an extra point of damage.</t>
+  </si>
+  <si>
+    <t>Shrouded (X) is a Damage Migration Test that may be taken in addition to a Saving Throw.</t>
+  </si>
+  <si>
+    <t>Skyfire</t>
+  </si>
+  <si>
+    <t>Attacks made with the Skyfire Special Rule ignore penalties when attacking Flyers.</t>
+  </si>
+  <si>
+    <t>Stun (X)</t>
+  </si>
+  <si>
+    <t>Weapons and other attacks that have the Stun (X) Special Rule have a chance of inflicting the Stunned Status on the Target Unit.</t>
+  </si>
+  <si>
+    <t>Support Unit (X)</t>
+  </si>
+  <si>
+    <t>A Unit that includes Models with this Special Rule scores fewer Victory Points for controlling Objective Markers.</t>
+  </si>
+  <si>
+    <t>Outflank</t>
+  </si>
+  <si>
+    <t>Panic (X)</t>
+  </si>
+  <si>
+    <t>Phage (X)</t>
+  </si>
+  <si>
+    <t>Pinning (X)</t>
+  </si>
+  <si>
+    <t>Pistol</t>
+  </si>
+  <si>
+    <t>Poisoned (X)</t>
+  </si>
+  <si>
+    <t>Precision (X)</t>
+  </si>
+  <si>
+    <t>trait</t>
+  </si>
+  <si>
+    <t>A Unit of Models with the Outflank Special Rule can enter play from outside of Deployment Zones.</t>
+  </si>
+  <si>
+    <t>Weapons and other attacks that have the Panic (X) Special Rule have a chance of inflicting the Routed Status on the Target Unit.</t>
+  </si>
+  <si>
+    <t>Unsaved Wounds with the Phage (X) Special Rule reduce a Characteristic by 1.</t>
+  </si>
+  <si>
+    <t>Weapons and other attacks that have the Pinning (X) Special Rule have a chance of inflicting the Pinned Status on the Target Unit.</t>
+  </si>
+  <si>
+    <t>A Model may attack with two Weapons that have the Pistol Special Rule.</t>
+  </si>
+  <si>
+    <t>A Weapon with the Poisoned (X) Special Rule has a chance to cause a wound regardless of the target's Toughness.</t>
+  </si>
+  <si>
+    <t>Attacks made with the Precision (X) Special Rule are allocated by the Attacking Player, not the Defender.</t>
+  </si>
+  <si>
+    <t>Heedless</t>
+  </si>
+  <si>
+    <t>Impact (X)</t>
+  </si>
+  <si>
+    <t>Infiltrate (X)</t>
+  </si>
+  <si>
+    <t>Light Transport</t>
+  </si>
+  <si>
+    <t>Models with this Special Rule cannot carry models with the Bulky (X) Special Rule.</t>
+  </si>
+  <si>
+    <t>Limited (X)</t>
+  </si>
+  <si>
+    <t>Line (X)</t>
+  </si>
+  <si>
+    <t>Move Through Cover</t>
+  </si>
+  <si>
+    <t>Officer of the Line (X)</t>
+  </si>
+  <si>
+    <t>Models with this Special Rule allow more Auxillary Detachments to be included in an Army.</t>
+  </si>
+  <si>
+    <t>Ordnance (X)</t>
+  </si>
+  <si>
+    <t>Weapons with the Ordnance (X) Special Rule double the value of a Characteristic when Stationary.</t>
+  </si>
+  <si>
+    <t>The Move Through Cover Special Rule allows the penalties of terrain to be ignored.</t>
+  </si>
+  <si>
+    <t>A Unit of Models with this Special Rule can control Objectives more easily and scores more Victory Points from controlling an Objective.</t>
+  </si>
+  <si>
+    <t>A Weapon with the Limited (X) Special Rule can only be used to attack a limited number of times per Battle.</t>
+  </si>
+  <si>
+    <t>Models with the Infiltrate (X) Special Rule can deploy outside of their Deployment Zone.</t>
+  </si>
+  <si>
+    <t>On a successful Charge, a Model with the Impact (X) Special Rule temporarily increases a Characteristic by 1.</t>
+  </si>
+  <si>
+    <t>A Unit that includes any Models with this Special Rule cannot claim Objectives.</t>
+  </si>
+  <si>
+    <t>A Model with this Special Rule can explode and cause Hits to nearby Models and Units.</t>
+  </si>
+  <si>
+    <t>A Unit that only includes Mmodels with the Fast (X) Special Rule gains a bonus to Rush and Charge Moves.</t>
+  </si>
+  <si>
+    <t>Feel No Pain (X) is a Damage Mitigation Test that may be taken in addition to a Saving Throw.</t>
+  </si>
+  <si>
+    <t>Models near an enemy Model with the Fear (X) Special Rule must reduce their Advanced Characteristics.</t>
+  </si>
+  <si>
+    <t>The Hatred (X) Special Rule grants bonuses against enemies of a specific Faction, Type or Trait.</t>
+  </si>
+  <si>
+    <t>A Weapon with this Special Rule may double a Characteristic with a Willpower Check, but may suffer Perils of the Warp.</t>
+  </si>
+  <si>
+    <t>Weapons with the Heavy (X) Special Rule gain _1 to a Characteristic when Stationary.</t>
+  </si>
+  <si>
+    <t>A Model with the Firing Protocols (X) Special Rule may attack with more than one ranged weapon.</t>
+  </si>
+  <si>
+    <t>Liber</t>
+  </si>
+  <si>
+    <t>Models with the Bulky (X) Special Rule take up more space on Transport Models.</t>
+  </si>
+  <si>
+    <t>Attacks made with the Critical Hit (X) Special Rule have a chance to automatically cause a wound and inflict 1 extra point of damage.</t>
+  </si>
+  <si>
+    <t>The Deep Strike Special Rule allows a Unit to enter play anywhere on the Battlefield.</t>
+  </si>
+  <si>
+    <t>Deflagrate (X)</t>
+  </si>
+  <si>
+    <t>Detonation</t>
+  </si>
+  <si>
+    <t>Duellist's Edge (X)</t>
+  </si>
+  <si>
+    <t>Eternal Warrior (X)</t>
+  </si>
+  <si>
+    <t>Expendable (X)</t>
+  </si>
+  <si>
+    <t>Unsaved Wounds inflicted by attacks with the Deflagrate (X) Special Rule can cause additional Hits.</t>
+  </si>
+  <si>
+    <t>Weapons with this Special Rule can only attack Vehicles and immobile Models.</t>
+  </si>
+  <si>
+    <t>A Weapon with the Duellist's Edge (X) Special Rule grants a bonus to Focus Rolls in Challenges.</t>
+  </si>
+  <si>
+    <t>A Model with this Special Rule takes less Damage from attacks.</t>
+  </si>
+  <si>
+    <t>A Player scores less Victory Points when they destroy a Unit that includes only Models with this Special Rule.</t>
+  </si>
+  <si>
+    <t>Armourbane</t>
+  </si>
+  <si>
+    <t>Assault Vehicle</t>
+  </si>
+  <si>
+    <t>Auto-repair (X)</t>
+  </si>
+  <si>
+    <t>Battlesmith (X)</t>
+  </si>
+  <si>
+    <t>A Weapon with the Armourbane Special Rule counts Glancing Hits as Penetrating Hits.</t>
+  </si>
+  <si>
+    <t>A Vehicle with this Special Rule allows Models to Disembark and Charge without penalty.</t>
+  </si>
+  <si>
+    <t>A Model with this Special Rule has a bonus to Repair Tests to remove Statuses.</t>
+  </si>
+  <si>
+    <t>A Weapon with this Special Rule may be used to attack Target Units out of Line of Sight.</t>
+  </si>
+  <si>
+    <t>A Model with the Battlesmith (X) Special Rule can repair Vehicles, Automata and other mechanical Units.</t>
+  </si>
+  <si>
+    <t>Attacks made with the Blast (X) Special Rule use a Blast Marker to determine how many Hits are caused.</t>
+  </si>
+  <si>
+    <t>With a Weapon that has the Breaching (X) Special Rule there is a chance that a Wound Test may result I nthe Wound ignoring Armour Saves.</t>
+  </si>
+  <si>
+    <t>[astartes] legion-saturnine-praetor</t>
+  </si>
+  <si>
+    <t>Praetor in Saturnine Terminator Armour</t>
+  </si>
+  <si>
+    <t>OPT0028</t>
+  </si>
+  <si>
+    <t>OPT0029</t>
+  </si>
+  <si>
+    <t>OPT0030</t>
+  </si>
+  <si>
+    <t>OPT0031</t>
+  </si>
+  <si>
+    <t>OPT0032</t>
+  </si>
+  <si>
+    <t>OPT0033</t>
+  </si>
+  <si>
+    <t>OPT0034</t>
+  </si>
+  <si>
+    <t>Saturnine concussion hammer</t>
+  </si>
+  <si>
+    <t>Plasma Blaster</t>
+  </si>
+  <si>
+    <t>Saturnine teleportation transponder</t>
+  </si>
+  <si>
+    <t>['[astartes] legion-praetor', '[astartes] legion-saturnine-praetor', '[astartes] legion-cataphractii-praetor', '[astartes] legion-tartaros-praetor', '[astartes] legion-centurion', '[astartes] legion-cataphractii-centurion', '[astartes] legion-tartaros-centurion', '[astartes] legion-damocles-command-rhino', '[astartes] legion-tactical-squad', '[astartes] legion-despoiler-squad', '[astartes] legion-assault-squad', '[astartes] legion-breacher-squad', '[astartes] legion-rhino', '[astartes] legion-drop-pod', '[astartes] legion-termite-assault-drill']</t>
+  </si>
+  <si>
+    <t>['[iron-warriors] warlord-perturabo']</t>
+  </si>
+  <si>
+    <t>["[astartes] legion-praetor", "[astartes] legion-saturnine-praetor", "[astartes] legion-cataphractii-praetor", "[astartes] legion-tartaros-praetor"]</t>
+  </si>
+  <si>
+    <t>Praetor in Cataphractii Terminator Armour</t>
+  </si>
+  <si>
+    <t>Praetor in Tartaros Terminator Armour</t>
+  </si>
+  <si>
+    <t>Praetor in Artificer Armour</t>
+  </si>
+  <si>
+    <t>Centurion in Artificer Armour</t>
+  </si>
+  <si>
+    <t>Centurion in Cataphractii Terminator Armour</t>
+  </si>
+  <si>
+    <t>Centurion in Tartaros Terminator Armour</t>
+  </si>
+  <si>
+    <t>Cataphractii Terminator Squad</t>
+  </si>
+  <si>
+    <t>Tartaros Terminator Squad</t>
+  </si>
+  <si>
+    <t>Saturnine Terminator Squad</t>
+  </si>
+  <si>
+    <t>[astartes] legion-terminator-saturnine-squad</t>
+  </si>
+  <si>
+    <t>['[astartes] legion-terminator-saturnine-squad', '[astartes] legion-terminator-cataphractii-squad', '[astartes] legion-terminator-tartaros-squad']</t>
+  </si>
+  <si>
+    <t>Plasma Bombard</t>
+  </si>
+  <si>
+    <t>Twin heavy disintegrator</t>
+  </si>
+  <si>
+    <t>Particle Shredder</t>
+  </si>
+  <si>
+    <t>Two lightning claws</t>
+  </si>
+  <si>
+    <t>Tactical Squad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -782,6 +1179,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -914,7 +1317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1021,11 +1424,50 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1173,13 +1615,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>168120</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>349200</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1225,13 +1667,60 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>168120</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="181080" cy="261000"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5231409" y="401053"/>
+          <a:ext cx="181080" cy="261000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>168120</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="181080" cy="261000"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 1">
+        <xdr:cNvPr id="4" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
@@ -1588,11 +2077,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A4"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -1601,7 +2090,7 @@
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
@@ -1666,22 +2155,22 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="9" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>65</v>
+        <v>336</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G2" s="1">
         <v>120</v>
@@ -1711,25 +2200,25 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="9" t="s">
-        <v>144</v>
+        <v>319</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>66</v>
+        <v>320</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G3" s="1">
-        <v>135</v>
+        <v>200</v>
       </c>
       <c r="H3" s="9" t="b">
         <f>FALSE()</f>
@@ -1756,25 +2245,25 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="9" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>67</v>
+        <v>334</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G4" s="1">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="H4" s="9" t="b">
         <f>FALSE()</f>
@@ -1801,25 +2290,25 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="9" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>68</v>
+        <v>335</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="G5" s="1">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="H5" s="9" t="b">
         <f>FALSE()</f>
@@ -1846,25 +2335,25 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="9" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>69</v>
+        <v>337</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G6" s="1">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="H6" s="9" t="b">
         <f>FALSE()</f>
@@ -1891,25 +2380,25 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="9" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>70</v>
+        <v>338</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G7" s="1">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H7" s="9" t="b">
         <f>FALSE()</f>
@@ -1936,25 +2425,25 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="9" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E8" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="G8" s="1">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="H8" s="9" t="b">
         <f>FALSE()</f>
@@ -1981,25 +2470,25 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="9" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="G9" s="1">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="H9" s="9" t="b">
         <f>FALSE()</f>
@@ -2026,25 +2515,25 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="9" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G10" s="1">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="H10" s="9" t="b">
         <f>FALSE()</f>
@@ -2071,25 +2560,25 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="9" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G11" s="1">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="H11" s="9" t="b">
         <f>FALSE()</f>
@@ -2116,25 +2605,25 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="9" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G12" s="1">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="H12" s="9" t="b">
         <f>FALSE()</f>
@@ -2161,22 +2650,22 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="9" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G13" s="1">
         <v>115</v>
@@ -2206,25 +2695,25 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="9" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G14" s="1">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="H14" s="9" t="b">
         <f>FALSE()</f>
@@ -2251,25 +2740,25 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="9" t="s">
-        <v>156</v>
+        <v>343</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>77</v>
+        <v>342</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G15" s="1">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="H15" s="9" t="b">
         <f>FALSE()</f>
@@ -2296,25 +2785,25 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="9" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>83</v>
+        <v>340</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G16" s="1">
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="H16" s="9" t="b">
         <f>FALSE()</f>
@@ -2341,25 +2830,25 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="9" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>84</v>
+        <v>341</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G17" s="1">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="H17" s="9" t="b">
         <f>FALSE()</f>
@@ -2385,26 +2874,26 @@
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="32" t="s">
-        <v>159</v>
+      <c r="A18" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>85</v>
+        <v>95</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G18" s="1">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="H18" s="9" t="b">
         <f>FALSE()</f>
@@ -2430,26 +2919,26 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="32" t="s">
-        <v>160</v>
+      <c r="A19" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="F19" t="s">
-        <v>87</v>
+        <v>95</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="G19" s="1">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="H19" s="9" t="b">
         <f>FALSE()</f>
@@ -2475,26 +2964,26 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="9" t="s">
-        <v>161</v>
+      <c r="A20" s="32" t="s">
+        <v>146</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" t="s">
-        <v>180</v>
+        <v>95</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="G20" s="1">
-        <v>175</v>
+        <v>45</v>
       </c>
       <c r="H20" s="9" t="b">
         <f>FALSE()</f>
@@ -2520,26 +3009,26 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="9" t="s">
-        <v>162</v>
+      <c r="A21" s="32" t="s">
+        <v>147</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>87</v>
+        <v>95</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" t="s">
+        <v>79</v>
       </c>
       <c r="G21" s="1">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="H21" s="9" t="b">
         <f>FALSE()</f>
@@ -2566,25 +3055,25 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="9" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>92</v>
+        <v>82</v>
+      </c>
+      <c r="F22" t="s">
+        <v>164</v>
       </c>
       <c r="G22" s="1">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="H22" s="9" t="b">
         <f>FALSE()</f>
@@ -2611,25 +3100,25 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="9" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G23" s="1">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="H23" s="9" t="b">
         <f>FALSE()</f>
@@ -2656,25 +3145,25 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="9" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>94</v>
+        <v>349</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G24" s="1">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="H24" s="9" t="b">
         <f>FALSE()</f>
@@ -2701,25 +3190,25 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="9" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G25" s="1">
-        <v>155</v>
+        <v>100</v>
       </c>
       <c r="H25" s="9" t="b">
         <f>FALSE()</f>
@@ -2746,25 +3235,25 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="9" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G26" s="1">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="H26" s="9" t="b">
         <f>FALSE()</f>
@@ -2791,25 +3280,25 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="9" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="G27" s="1">
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="H27" s="9" t="b">
         <f>FALSE()</f>
@@ -2836,25 +3325,25 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="9" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="G28" s="1">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="H28" s="9" t="b">
         <f>FALSE()</f>
@@ -2881,25 +3370,25 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="9" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G29" s="1">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="H29" s="9" t="b">
         <f>FALSE()</f>
@@ -2926,25 +3415,25 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="9" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G30" s="1">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="H30" s="9" t="b">
         <f>FALSE()</f>
@@ -2971,25 +3460,25 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="9" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="G31" s="1">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="H31" s="9" t="b">
         <f>FALSE()</f>
@@ -3016,25 +3505,25 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="9" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="G32" s="1">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="H32" s="9" t="b">
         <f>FALSE()</f>
@@ -3059,8 +3548,188 @@
         <v>16</v>
       </c>
     </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G33" s="1">
+        <v>100</v>
+      </c>
+      <c r="H33" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0</v>
+      </c>
+      <c r="L33" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34" s="1">
+        <v>80</v>
+      </c>
+      <c r="H34" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="9">
+        <v>0</v>
+      </c>
+      <c r="L34" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G35" s="1">
+        <v>600</v>
+      </c>
+      <c r="H35" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="9">
+        <v>0</v>
+      </c>
+      <c r="L35" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G36" s="1">
+        <v>400</v>
+      </c>
+      <c r="H36" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="9">
+        <v>0</v>
+      </c>
+      <c r="L36" s="9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P36" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:P32"/>
+  <autoFilter ref="A1:P34"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -3073,7 +3742,7 @@
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -3124,16 +3793,16 @@
         <v>24</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D2" s="33">
         <v>2</v>
       </c>
-      <c r="E2" s="35" t="s">
-        <v>110</v>
+      <c r="E2" s="38" t="s">
+        <v>100</v>
       </c>
       <c r="F2" s="33"/>
       <c r="G2" s="34"/>
@@ -3145,16 +3814,16 @@
         <v>25</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D3" s="33">
         <v>10</v>
       </c>
-      <c r="E3" s="35" t="s">
-        <v>110</v>
+      <c r="E3" s="38" t="s">
+        <v>100</v>
       </c>
       <c r="F3" s="33"/>
       <c r="G3" s="34"/>
@@ -3166,16 +3835,16 @@
         <v>26</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D4" s="33">
         <v>5</v>
       </c>
-      <c r="E4" s="35" t="s">
-        <v>110</v>
+      <c r="E4" s="38" t="s">
+        <v>100</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
@@ -3187,16 +3856,16 @@
         <v>27</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D5" s="33">
         <v>2</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>110</v>
+      <c r="E5" s="38" t="s">
+        <v>100</v>
       </c>
       <c r="F5" s="33"/>
       <c r="G5" s="34"/>
@@ -3208,16 +3877,16 @@
         <v>28</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D6" s="33">
         <v>2</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>110</v>
+      <c r="E6" s="38" t="s">
+        <v>100</v>
       </c>
       <c r="F6" s="33"/>
       <c r="G6" s="34"/>
@@ -3229,16 +3898,16 @@
         <v>29</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D7" s="33">
         <v>10</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>110</v>
+      <c r="E7" s="38" t="s">
+        <v>100</v>
       </c>
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
@@ -3250,16 +3919,16 @@
         <v>30</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D8" s="33">
         <v>2</v>
       </c>
-      <c r="E8" s="35" t="s">
-        <v>125</v>
+      <c r="E8" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F8" s="33"/>
       <c r="G8" s="34"/>
@@ -3271,16 +3940,16 @@
         <v>31</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D9" s="33">
         <v>2</v>
       </c>
-      <c r="E9" s="35" t="s">
-        <v>125</v>
+      <c r="E9" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F9" s="33"/>
       <c r="G9" s="34"/>
@@ -3292,16 +3961,16 @@
         <v>32</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D10" s="33">
         <v>10</v>
       </c>
-      <c r="E10" s="35" t="s">
-        <v>125</v>
+      <c r="E10" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F10" s="33"/>
       <c r="G10" s="34"/>
@@ -3313,16 +3982,16 @@
         <v>33</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D11" s="33">
         <v>15</v>
       </c>
-      <c r="E11" s="35" t="s">
-        <v>125</v>
+      <c r="E11" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F11" s="33"/>
       <c r="G11" s="34"/>
@@ -3334,16 +4003,16 @@
         <v>34</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D12" s="33">
         <v>20</v>
       </c>
-      <c r="E12" s="35" t="s">
-        <v>125</v>
+      <c r="E12" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F12" s="33"/>
       <c r="G12" s="34"/>
@@ -3355,16 +4024,16 @@
         <v>35</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D13" s="33">
         <v>5</v>
       </c>
-      <c r="E13" s="35" t="s">
-        <v>125</v>
+      <c r="E13" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F13" s="33"/>
       <c r="G13" s="34"/>
@@ -3376,16 +4045,16 @@
         <v>36</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D14" s="33">
         <v>10</v>
       </c>
-      <c r="E14" s="35" t="s">
-        <v>125</v>
+      <c r="E14" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F14" s="33"/>
       <c r="G14" s="34"/>
@@ -3397,16 +4066,16 @@
         <v>37</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D15" s="33">
         <v>15</v>
       </c>
-      <c r="E15" s="35" t="s">
-        <v>125</v>
+      <c r="E15" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F15" s="33"/>
       <c r="G15" s="34"/>
@@ -3418,16 +4087,16 @@
         <v>38</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D16" s="33">
         <v>25</v>
       </c>
-      <c r="E16" s="35" t="s">
-        <v>125</v>
+      <c r="E16" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F16" s="33"/>
       <c r="G16" s="34"/>
@@ -3439,16 +4108,16 @@
         <v>39</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D17" s="33">
         <v>10</v>
       </c>
-      <c r="E17" s="35" t="s">
-        <v>125</v>
+      <c r="E17" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F17" s="33"/>
       <c r="G17" s="34"/>
@@ -3460,16 +4129,16 @@
         <v>40</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D18" s="10">
         <v>30</v>
       </c>
-      <c r="E18" s="35" t="s">
-        <v>125</v>
+      <c r="E18" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F18" s="33"/>
       <c r="G18" s="34"/>
@@ -3481,16 +4150,16 @@
         <v>41</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D19" s="33">
         <v>30</v>
       </c>
-      <c r="E19" s="35" t="s">
-        <v>125</v>
+      <c r="E19" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F19" s="33"/>
       <c r="G19" s="34"/>
@@ -3502,16 +4171,16 @@
         <v>42</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D20" s="33">
         <v>0</v>
       </c>
-      <c r="E20" s="35" t="s">
-        <v>125</v>
+      <c r="E20" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="F20" s="33"/>
       <c r="G20" s="34"/>
@@ -3523,16 +4192,16 @@
         <v>43</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>106</v>
+        <v>348</v>
       </c>
       <c r="D21" s="33">
         <v>20</v>
       </c>
-      <c r="E21" s="35" t="s">
-        <v>118</v>
+      <c r="E21" s="38" t="s">
+        <v>108</v>
       </c>
       <c r="F21" s="33"/>
       <c r="G21" s="34"/>
@@ -3544,16 +4213,16 @@
         <v>44</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D22" s="33">
         <v>0</v>
       </c>
-      <c r="E22" s="35" t="s">
-        <v>110</v>
+      <c r="E22" s="38" t="s">
+        <v>100</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="34"/>
@@ -3565,16 +4234,16 @@
         <v>45</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D23" s="33">
         <v>10</v>
       </c>
-      <c r="E23" s="35" t="s">
-        <v>110</v>
+      <c r="E23" s="38" t="s">
+        <v>100</v>
       </c>
       <c r="F23" s="33"/>
       <c r="G23" s="34"/>
@@ -3586,16 +4255,16 @@
         <v>46</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D24" s="33">
         <v>10</v>
       </c>
-      <c r="E24" s="35" t="s">
-        <v>110</v>
+      <c r="E24" s="38" t="s">
+        <v>100</v>
       </c>
       <c r="F24" s="33"/>
       <c r="G24" s="34"/>
@@ -3607,20 +4276,22 @@
         <v>47</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D25" s="33">
         <v>20</v>
       </c>
-      <c r="E25" s="35"/>
+      <c r="E25" s="38" t="s">
+        <v>196</v>
+      </c>
       <c r="F25" s="33"/>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
       <c r="I25" s="33" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -3628,20 +4299,22 @@
         <v>48</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D26" s="33">
         <v>20</v>
       </c>
-      <c r="E26" s="33"/>
+      <c r="E26" s="38" t="s">
+        <v>196</v>
+      </c>
       <c r="F26" s="33"/>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
       <c r="I26" s="34" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -3649,94 +4322,166 @@
         <v>49</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D27" s="33">
         <v>30</v>
       </c>
-      <c r="E27" s="33"/>
+      <c r="E27" s="38" t="s">
+        <v>196</v>
+      </c>
       <c r="F27" s="33"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="33"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
+      <c r="A28" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>328</v>
+      </c>
+      <c r="D28" s="33">
+        <v>10</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>115</v>
+      </c>
       <c r="F28" s="33"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="33"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
+      <c r="A29" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="D29" s="33">
+        <v>10</v>
+      </c>
+      <c r="E29" s="38" t="s">
+        <v>100</v>
+      </c>
       <c r="F29" s="33"/>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="33"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
+      <c r="A30" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>330</v>
+      </c>
+      <c r="D30" s="33">
+        <v>60</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>100</v>
+      </c>
       <c r="F30" s="33"/>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="33"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
+      <c r="A31" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>345</v>
+      </c>
+      <c r="D31" s="33">
+        <v>0</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>115</v>
+      </c>
       <c r="F31" s="33"/>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="33"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
+      <c r="A32" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="D32" s="33">
+        <v>10</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>115</v>
+      </c>
       <c r="F32" s="33"/>
       <c r="G32" s="34"/>
       <c r="H32" s="34"/>
       <c r="I32" s="34"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="33"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
+      <c r="A33" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="D33" s="33">
+        <v>10</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>115</v>
+      </c>
       <c r="F33" s="33"/>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
       <c r="I33" s="34"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="33"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
+      <c r="A34" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>347</v>
+      </c>
+      <c r="D34" s="33">
+        <v>5</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>100</v>
+      </c>
       <c r="F34" s="33"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
@@ -19199,7 +19944,7 @@
   <autoFilter ref="A1:I1387"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -19208,11 +19953,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -19223,7 +19968,7 @@
     <col min="4" max="4" width="95.140625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>4</v>
       </c>
@@ -19237,409 +19982,808 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45">
+    <row r="2" spans="1:5">
       <c r="A2" s="16" t="s">
-        <v>174</v>
+        <v>217</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="10"/>
-      <c r="D2" s="16" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45">
+      <c r="D2" s="16"/>
+      <c r="E2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45">
       <c r="A3" s="16" t="s">
-        <v>136</v>
+        <v>216</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45">
-      <c r="A4" s="10" t="s">
-        <v>135</v>
+        <v>205</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45">
+      <c r="A4" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>207</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="10" t="s">
-        <v>194</v>
+        <v>125</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="16" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="B6" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="18" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="B7" s="16" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="18" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="B8" s="16" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="37" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="B9" s="16" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="16"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="18"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="16"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="16"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="36" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>308</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>309</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="18" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" t="s">
+        <v>311</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="16"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="18"/>
+      <c r="D16" s="16" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30">
+      <c r="A17" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="16" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
+      <c r="A18" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
+      <c r="D18" s="16" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30">
+      <c r="A19" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="16"/>
+      <c r="D19" s="16" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="16"/>
+      <c r="A20" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="18" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
+      <c r="A21" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="18"/>
+      <c r="D21" s="18" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="16"/>
+      <c r="A22" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="18" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="18" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="18"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
+      <c r="D24" s="18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30">
+      <c r="A25" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C25" s="9"/>
-      <c r="D25" s="18"/>
+      <c r="D25" s="18" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="16"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="18"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="18"/>
+      <c r="A26" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30">
+      <c r="A27" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="16" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30">
+      <c r="A28" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="16" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="16"/>
+      <c r="A29" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="18" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
+      <c r="A30" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C30" s="9"/>
-      <c r="D30" s="18"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="16"/>
+      <c r="D30" s="18" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30">
+      <c r="A31" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="18" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="18"/>
+      <c r="A32" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="16" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="18"/>
+      <c r="A33" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="16" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
+      <c r="A34" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C34" s="10"/>
-      <c r="D34" s="16"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="18"/>
+      <c r="D34" s="16" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30">
+      <c r="A35" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="16" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="16"/>
+      <c r="A36" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="18" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C37" s="10"/>
-      <c r="D37" s="16"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
+      <c r="D37" s="16" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30">
+      <c r="A38" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C38" s="10"/>
-      <c r="D38" s="16"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
+      <c r="D38" s="16" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30">
+      <c r="A39" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C39" s="10"/>
-      <c r="D39" s="16"/>
+      <c r="D39" s="16" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C40" s="10"/>
-      <c r="D40" s="16"/>
+      <c r="D40" s="16" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="18"/>
+      <c r="A41" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="16" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
+      <c r="A42" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C42" s="10"/>
-      <c r="D42" s="16"/>
+      <c r="D42" s="16" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="18"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
+      <c r="A43" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="30">
+      <c r="A44" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C44" s="10"/>
-      <c r="D44" s="16"/>
+      <c r="D44" s="16" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
+      <c r="A45" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C45" s="10"/>
-      <c r="D45" s="16"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="16"/>
+      <c r="D45" s="16" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30">
+      <c r="A46" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="16" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="18"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="16"/>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
+      <c r="A47" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30">
+      <c r="A48" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="16" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30">
+      <c r="A49" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C49" s="10"/>
-      <c r="D49" s="16"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
+      <c r="D49" s="16" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C50" s="10"/>
-      <c r="D50" s="16"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
+      <c r="D50" s="16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30">
+      <c r="A51" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C51" s="10"/>
-      <c r="D51" s="16"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="16"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="16"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="18"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="16"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
+      <c r="D51" s="16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30">
+      <c r="A52" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="18" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" s="10"/>
+      <c r="D54" s="16" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="18" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30">
+      <c r="A56" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C56" s="10"/>
-      <c r="D56" s="16"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="16"/>
+      <c r="D56" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="30">
+      <c r="A57" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" s="10"/>
+      <c r="D57" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30">
+      <c r="A58" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" s="18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30">
+      <c r="A59" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C59" s="10"/>
+      <c r="D59" s="16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C61" s="10"/>
+      <c r="D61" s="16"/>
+      <c r="E61" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="18"/>
+      <c r="E62" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="10"/>
+      <c r="D63" s="16"/>
+      <c r="E63" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="10"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="16"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="10"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="16"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="10"/>
+      <c r="B66" s="10"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D49">
+  <autoFilter ref="A1:D38">
     <sortState ref="A2:D149">
       <sortCondition ref="A2:A149"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A4:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  <conditionalFormatting sqref="A16:A20 A14 A1 A5:A10 A25:A1048576">
+    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+  <conditionalFormatting sqref="D9">
+    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
     <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -19649,7 +20793,7 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -19691,13 +20835,13 @@
     </row>
     <row r="2" spans="1:8" ht="120">
       <c r="A2" s="10" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D2" s="10">
         <v>0</v>
@@ -19706,7 +20850,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="210">
@@ -19717,7 +20861,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="D3" s="10">
         <v>0</v>
@@ -20401,7 +21545,7 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -20424,10 +21568,10 @@
     </row>
     <row r="2" spans="1:3" ht="60">
       <c r="A2" s="9" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>212</v>
+        <v>331</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>16</v>
@@ -20435,10 +21579,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="9" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>16</v>
@@ -20446,10 +21590,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="9" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>16</v>
@@ -20457,10 +21601,10 @@
     </row>
     <row r="5" spans="1:3" ht="29.25" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>16</v>
@@ -20468,7 +21612,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="9" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>16</v>
@@ -20476,10 +21620,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>16</v>
@@ -20487,7 +21631,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="9" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>16</v>
@@ -20495,10 +21639,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="9" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>16</v>
@@ -20506,10 +21650,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="9" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>16</v>
@@ -20517,10 +21661,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="9" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>178</v>
+        <v>344</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>16</v>
@@ -20528,7 +21672,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="9" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>16</v>
@@ -20536,7 +21680,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="9" t="s">
-        <v>191</v>
+        <v>175</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>332</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>16</v>
@@ -20544,7 +21691,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="9" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>16</v>
@@ -20552,7 +21699,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="9" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>16</v>
@@ -20581,8 +21728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C15" sqref="C14:C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -20610,44 +21757,44 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="17" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="25.5">
       <c r="A3" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>213</v>
+        <v>333</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="38.25">
       <c r="A4" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>63</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>

<commit_message>
fixing python script problems, then types
</commit_message>
<xml_diff>
--- a/data/hh3_data.xlsx
+++ b/data/hh3_data.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="388">
   <si>
     <t>model_id</t>
   </si>
@@ -1062,13 +1062,7 @@
     <t>traits</t>
   </si>
   <si>
-    <t>Crusade</t>
-  </si>
-  <si>
     <t>First Strike</t>
-  </si>
-  <si>
-    <t>Allied</t>
   </si>
   <si>
     <t>May select a Rite of War. May select one Apex Detachment.</t>
@@ -2194,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -2204,7 +2198,7 @@
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
@@ -2241,7 +2235,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>95</v>
@@ -2256,7 +2250,7 @@
         <v>293</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>332</v>
+        <v>293</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
@@ -2272,7 +2266,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>95</v>
@@ -2287,7 +2281,7 @@
         <v>294</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>58</v>
+        <v>294</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -2299,7 +2293,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>95</v>
@@ -2314,7 +2308,7 @@
         <v>296</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>57</v>
+        <v>296</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -2326,7 +2320,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>95</v>
@@ -2341,7 +2335,7 @@
         <v>295</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>342</v>
+        <v>295</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -2353,7 +2347,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>95</v>
@@ -2367,8 +2361,8 @@
       <c r="E6" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="F6" s="34" t="s">
-        <v>63</v>
+      <c r="F6" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -2380,7 +2374,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>95</v>
@@ -2395,7 +2389,7 @@
         <v>298</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>60</v>
+        <v>298</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -2407,7 +2401,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>95</v>
@@ -2421,8 +2415,8 @@
       <c r="E8" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="F8" s="34" t="s">
-        <v>341</v>
+      <c r="F8" s="7" t="s">
+        <v>299</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -2434,7 +2428,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>95</v>
@@ -2449,7 +2443,7 @@
         <v>300</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>128</v>
+        <v>300</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -2461,7 +2455,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>95</v>
@@ -2476,7 +2470,7 @@
         <v>301</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>62</v>
+        <v>301</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -2488,7 +2482,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>95</v>
@@ -2503,7 +2497,7 @@
         <v>302</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>59</v>
+        <v>302</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -2515,7 +2509,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>95</v>
@@ -2530,7 +2524,7 @@
         <v>303</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>333</v>
+        <v>303</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -2542,7 +2536,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>95</v>
@@ -2557,7 +2551,7 @@
         <v>304</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>149</v>
+        <v>304</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -2569,7 +2563,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>95</v>
@@ -2584,7 +2578,7 @@
         <v>305</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>152</v>
+        <v>305</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -2596,7 +2590,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>95</v>
@@ -2611,7 +2605,7 @@
         <v>306</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>334</v>
+        <v>306</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -2935,7 +2929,7 @@
         <v>311</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G27" s="1">
         <v>115</v>
@@ -2962,7 +2956,7 @@
         <v>312</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G28" s="1">
         <v>115</v>
@@ -3070,7 +3064,7 @@
         <v>313</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G32" s="1">
         <v>130</v>
@@ -3097,7 +3091,7 @@
         <v>314</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G33" s="1">
         <v>105</v>
@@ -3121,7 +3115,7 @@
         <v>64</v>
       </c>
       <c r="E34" s="34" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>60</v>
@@ -3148,7 +3142,7 @@
         <v>64</v>
       </c>
       <c r="E35" s="34" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F35" t="s">
         <v>60</v>
@@ -3568,7 +3562,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>95</v>
@@ -3580,10 +3574,10 @@
         <v>64</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G51" s="1">
         <v>80</v>
@@ -3595,7 +3589,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>95</v>
@@ -3607,10 +3601,10 @@
         <v>64</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G52" s="1">
         <v>75</v>
@@ -3622,7 +3616,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>95</v>
@@ -3634,7 +3628,7 @@
         <v>64</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>128</v>
@@ -3657,10 +3651,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ1577"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -4407,13 +4401,13 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="30" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D35" s="30">
         <v>10</v>
@@ -4428,13 +4422,13 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="30" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D36" s="30">
         <v>10</v>
@@ -4449,13 +4443,13 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="30" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D37" s="30">
         <v>10</v>
@@ -4470,13 +4464,13 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="30" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D38" s="30">
         <v>0</v>
@@ -4491,13 +4485,13 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="30" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D39" s="30">
         <v>0</v>
@@ -4512,13 +4506,13 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="30" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D40" s="30">
         <v>0</v>
@@ -4533,13 +4527,13 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="30" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D41" s="30">
         <v>10</v>
@@ -4554,13 +4548,13 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="30" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D42" s="30">
         <v>10</v>
@@ -19955,7 +19949,7 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -19989,7 +19983,7 @@
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="33" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
@@ -20001,7 +19995,7 @@
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="33" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E3" s="14"/>
     </row>
@@ -20014,7 +20008,7 @@
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="33" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E4" s="14"/>
     </row>
@@ -20027,24 +20021,24 @@
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="33" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="32" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B6" s="33" t="s">
         <v>331</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="33" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>12</v>
@@ -20064,7 +20058,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>12</v>
@@ -20072,7 +20066,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>12</v>
@@ -20082,7 +20076,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>12</v>
@@ -20768,7 +20762,7 @@
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="16" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E68" t="s">
         <v>237</v>
@@ -20812,7 +20806,7 @@
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -20826,7 +20820,7 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -20859,7 +20853,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>9</v>
@@ -21338,10 +21332,10 @@
   </sheetData>
   <autoFilter ref="A1:D108"/>
   <conditionalFormatting sqref="A107:A1048576 A1 A3:A105">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -21354,7 +21348,7 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -21377,7 +21371,7 @@
     </row>
     <row r="2" spans="1:3" ht="60">
       <c r="A2" s="7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>274</v>
@@ -21388,7 +21382,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>154</v>
@@ -21399,7 +21393,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>141</v>
@@ -21410,7 +21404,7 @@
     </row>
     <row r="5" spans="1:3" ht="29.25" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>129</v>
@@ -21421,10 +21415,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>9</v>
@@ -21432,7 +21426,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>143</v>
@@ -21443,10 +21437,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>9</v>
@@ -21454,10 +21448,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>9</v>
@@ -21465,7 +21459,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>142</v>
@@ -21476,7 +21470,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>287</v>
@@ -21487,10 +21481,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>9</v>
@@ -21498,7 +21492,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>275</v>
@@ -21509,10 +21503,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>9</v>
@@ -21520,7 +21514,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>141</v>
@@ -21552,8 +21546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="C1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="C46" sqref="C42:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fixed data and ran python
</commit_message>
<xml_diff>
--- a/data/hh3_data.xlsx
+++ b/data/hh3_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-3345" yWindow="10695" windowWidth="25815" windowHeight="15495" tabRatio="500"/>
+    <workbookView xWindow="-3345" yWindow="10695" windowWidth="25815" windowHeight="15495" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">army_lists!$A$1:$D$108</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">hero_constraints!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">keywords!$A$1:$D$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">keywords!$A$1:$C$44</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">models!$A$1:$I$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">options!$A$1:$I$1387</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">warning_rules!$A$1:$D$1</definedName>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="386">
   <si>
     <t>model_id</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>OPT0027</t>
-  </si>
-  <si>
-    <t>active_passive</t>
   </si>
   <si>
     <t>description</t>
@@ -777,9 +774,6 @@
     <t>A Model with the Firing Protocols (X) Special Rule may attack with more than one ranged weapon.</t>
   </si>
   <si>
-    <t>Liber</t>
-  </si>
-  <si>
     <t>Models with the Bulky (X) Special Rule take up more space on Transport Models.</t>
   </si>
   <si>
@@ -1111,128 +1105,128 @@
   </si>
   <si>
     <t>With a Weapon that has the Overload (X) Special Rule, there is a chance that a Hit Test may result in an automatic wound to the user.</t>
+  </si>
+  <si>
+    <t>['[astartes] legion-rhino', '[astartes] legion-drop-pod', '[astartes] legion-termite-assault-drill']</t>
+  </si>
+  <si>
+    <t>jetbike-squad</t>
+  </si>
+  <si>
+    <t>Jetbike Squad</t>
+  </si>
+  <si>
+    <t>['jetbike-squad']</t>
+  </si>
+  <si>
+    <t>[detachment] crusade-primary-detachment</t>
+  </si>
+  <si>
+    <t>[detachment] combat-retinue</t>
+  </si>
+  <si>
+    <t>[detachment] officer-cadre</t>
+  </si>
+  <si>
+    <t>[detachment] army-vanguard</t>
+  </si>
+  <si>
+    <t>[detachment] armoured-fist</t>
+  </si>
+  <si>
+    <t>[detachment] tactical-support</t>
+  </si>
+  <si>
+    <t>[detachment] armoured-support</t>
+  </si>
+  <si>
+    <t>[detachment] heavy-support</t>
+  </si>
+  <si>
+    <t>[detachment] combat-pioneers</t>
+  </si>
+  <si>
+    <t>[detachment] shock-assault</t>
+  </si>
+  <si>
+    <t>[detachment] first-strike</t>
+  </si>
+  <si>
+    <t>[detachment] warlord</t>
+  </si>
+  <si>
+    <t>[detachment] lord-of-war</t>
+  </si>
+  <si>
+    <t>[detachment] allied-detachment</t>
+  </si>
+  <si>
+    <t>saturnine-dreadnought</t>
+  </si>
+  <si>
+    <t>Saturnine Dreadnought</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>Smokescreen</t>
+  </si>
+  <si>
+    <t>This does something with smoke.</t>
+  </si>
+  <si>
+    <t>OPT0035</t>
+  </si>
+  <si>
+    <t>OPT0036</t>
+  </si>
+  <si>
+    <t>OPT0037</t>
+  </si>
+  <si>
+    <t>OPT0038</t>
+  </si>
+  <si>
+    <t>OPT0039</t>
+  </si>
+  <si>
+    <t>OPT0040</t>
+  </si>
+  <si>
+    <t>OPT0041</t>
+  </si>
+  <si>
+    <t>Disintegrator cannon</t>
+  </si>
+  <si>
+    <t>Inversion beamer</t>
+  </si>
+  <si>
+    <t>Graviton pulveriser</t>
+  </si>
+  <si>
+    <t>Heavy plasma bombard</t>
+  </si>
+  <si>
+    <t>Two concussive resonators</t>
+  </si>
+  <si>
+    <t>Two heavy particle shredders</t>
+  </si>
+  <si>
+    <t>OPT0042</t>
+  </si>
+  <si>
+    <t>['[astartes] legion-contemptor-dreadnought', 'saturnine-dreadnought']</t>
   </si>
   <si>
     <t>[
     {
-        "title": "\"Placeholder"\",
+        "title": "\"Placeholder\"",
         "description": "And they shall know no fear."
     },
 ]</t>
-  </si>
-  <si>
-    <t>['[astartes] legion-rhino', '[astartes] legion-drop-pod', '[astartes] legion-termite-assault-drill']</t>
-  </si>
-  <si>
-    <t>jetbike-squad</t>
-  </si>
-  <si>
-    <t>Jetbike Squad</t>
-  </si>
-  <si>
-    <t>['jetbike-squad']</t>
-  </si>
-  <si>
-    <t>[detachment] crusade-primary-detachment</t>
-  </si>
-  <si>
-    <t>[detachment] combat-retinue</t>
-  </si>
-  <si>
-    <t>[detachment] officer-cadre</t>
-  </si>
-  <si>
-    <t>[detachment] army-vanguard</t>
-  </si>
-  <si>
-    <t>[detachment] armoured-fist</t>
-  </si>
-  <si>
-    <t>[detachment] tactical-support</t>
-  </si>
-  <si>
-    <t>[detachment] armoured-support</t>
-  </si>
-  <si>
-    <t>[detachment] heavy-support</t>
-  </si>
-  <si>
-    <t>[detachment] combat-pioneers</t>
-  </si>
-  <si>
-    <t>[detachment] shock-assault</t>
-  </si>
-  <si>
-    <t>[detachment] first-strike</t>
-  </si>
-  <si>
-    <t>[detachment] warlord</t>
-  </si>
-  <si>
-    <t>[detachment] lord-of-war</t>
-  </si>
-  <si>
-    <t>[detachment] allied-detachment</t>
-  </si>
-  <si>
-    <t>saturnine-dreadnought</t>
-  </si>
-  <si>
-    <t>Saturnine Dreadnought</t>
-  </si>
-  <si>
-    <t>Walker</t>
-  </si>
-  <si>
-    <t>Smokescreen</t>
-  </si>
-  <si>
-    <t>This does something with smoke.</t>
-  </si>
-  <si>
-    <t>OPT0035</t>
-  </si>
-  <si>
-    <t>OPT0036</t>
-  </si>
-  <si>
-    <t>OPT0037</t>
-  </si>
-  <si>
-    <t>OPT0038</t>
-  </si>
-  <si>
-    <t>OPT0039</t>
-  </si>
-  <si>
-    <t>OPT0040</t>
-  </si>
-  <si>
-    <t>OPT0041</t>
-  </si>
-  <si>
-    <t>Disintegrator cannon</t>
-  </si>
-  <si>
-    <t>Inversion beamer</t>
-  </si>
-  <si>
-    <t>Graviton pulveriser</t>
-  </si>
-  <si>
-    <t>Heavy plasma bombard</t>
-  </si>
-  <si>
-    <t>Two concussive resonators</t>
-  </si>
-  <si>
-    <t>Two heavy particle shredders</t>
-  </si>
-  <si>
-    <t>OPT0042</t>
-  </si>
-  <si>
-    <t>['[astartes] legion-contemptor-dreadnought', 'saturnine-dreadnought']</t>
   </si>
 </sst>
 </file>
@@ -1420,7 +1414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1529,6 +1523,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1721,13 +1724,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>168120</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>349200</xdr:colOff>
+      <xdr:colOff>181080</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
@@ -1736,7 +1739,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1773,7 +1776,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>168120</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1783,7 +1786,7 @@
         <xdr:cNvPr id="3" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1820,7 +1823,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>168120</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1830,7 +1833,7 @@
         <xdr:cNvPr id="4" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2176,7 +2179,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2186,9 +2189,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -2235,22 +2238,22 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="7" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
@@ -2266,22 +2269,22 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="7" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D3" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -2293,22 +2296,22 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="7" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -2320,22 +2323,22 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -2347,22 +2350,22 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="7" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -2374,22 +2377,22 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="7" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -2401,22 +2404,22 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="7" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -2428,22 +2431,22 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="7" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -2455,22 +2458,22 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="7" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D10" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -2482,22 +2485,22 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="7" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -2509,22 +2512,22 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="7" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D12" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -2536,22 +2539,22 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D13" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -2563,22 +2566,22 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="7" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D14" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -2590,22 +2593,22 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="7" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D15" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -2617,22 +2620,22 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D16" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G16" s="1">
         <v>120</v>
@@ -2644,22 +2647,22 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D17" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G17" s="1">
         <v>200</v>
@@ -2671,22 +2674,22 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D18" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G18" s="1">
         <v>135</v>
@@ -2698,22 +2701,22 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D19" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G19" s="1">
         <v>110</v>
@@ -2725,22 +2728,22 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D20" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20" s="1">
         <v>60</v>
@@ -2752,22 +2755,22 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D21" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G21" s="1">
         <v>85</v>
@@ -2779,22 +2782,22 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D22" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G22" s="1">
         <v>75</v>
@@ -2806,22 +2809,22 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D23" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G23" s="1">
         <v>85</v>
@@ -2833,22 +2836,22 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D24" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G24" s="1">
         <v>125</v>
@@ -2860,22 +2863,22 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D25" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G25" s="1">
         <v>110</v>
@@ -2887,22 +2890,22 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D26" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G26" s="1">
         <v>150</v>
@@ -2914,22 +2917,22 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D27" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G27" s="1">
         <v>115</v>
@@ -2941,22 +2944,22 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D28" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G28" s="1">
         <v>115</v>
@@ -2968,22 +2971,22 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D29" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G29" s="1">
         <v>175</v>
@@ -2995,22 +2998,22 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D30" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G30" s="1">
         <v>175</v>
@@ -3022,22 +3025,22 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D31" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G31" s="1">
         <v>150</v>
@@ -3049,22 +3052,22 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D32" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G32" s="1">
         <v>130</v>
@@ -3076,22 +3079,22 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D33" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G33" s="1">
         <v>105</v>
@@ -3103,22 +3106,22 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D34" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E34" s="34" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G34" s="1">
         <v>45</v>
@@ -3130,22 +3133,22 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D35" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E35" s="34" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G35" s="1">
         <v>55</v>
@@ -3157,22 +3160,22 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D36" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G36" s="1">
         <v>175</v>
@@ -3184,22 +3187,22 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D37" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E37" s="34" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G37" s="1">
         <v>40</v>
@@ -3211,22 +3214,22 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D38" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E38" s="34" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G38" s="1">
         <v>100</v>
@@ -3238,22 +3241,22 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D39" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G39" s="1">
         <v>100</v>
@@ -3265,22 +3268,22 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D40" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G40" s="1">
         <v>145</v>
@@ -3292,22 +3295,22 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D41" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G41" s="1">
         <v>155</v>
@@ -3319,22 +3322,22 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D42" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G42" s="1">
         <v>85</v>
@@ -3346,22 +3349,22 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D43" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G43" s="1">
         <v>85</v>
@@ -3373,22 +3376,22 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B44" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D44" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G44" s="1">
         <v>65</v>
@@ -3400,22 +3403,22 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D45" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G45" s="1">
         <v>35</v>
@@ -3427,22 +3430,22 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D46" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G46" s="1">
         <v>35</v>
@@ -3454,22 +3457,22 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D47" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G47" s="1">
         <v>100</v>
@@ -3481,22 +3484,22 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D48" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G48" s="1">
         <v>80</v>
@@ -3508,22 +3511,22 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="G49" s="1">
         <v>600</v>
@@ -3535,22 +3538,22 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E50" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F50" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="G50" s="1">
         <v>400</v>
@@ -3562,22 +3565,22 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="F51" s="7" t="s">
         <v>337</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>339</v>
       </c>
       <c r="G51" s="1">
         <v>80</v>
@@ -3589,22 +3592,22 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D52" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G52" s="1">
         <v>75</v>
@@ -3616,22 +3619,22 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B53" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C53" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="D53" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G53" s="1">
         <v>340</v>
@@ -3705,16 +3708,16 @@
         <v>17</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" s="30">
         <v>2</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="31"/>
@@ -3726,16 +3729,16 @@
         <v>18</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="30">
         <v>10</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="31"/>
@@ -3747,16 +3750,16 @@
         <v>19</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="30">
         <v>5</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="31"/>
@@ -3768,16 +3771,16 @@
         <v>20</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="30">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="30"/>
       <c r="G5" s="31"/>
@@ -3789,16 +3792,16 @@
         <v>21</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="30">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" s="30"/>
       <c r="G6" s="31"/>
@@ -3810,16 +3813,16 @@
         <v>22</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="30">
         <v>10</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" s="30"/>
       <c r="G7" s="31"/>
@@ -3831,16 +3834,16 @@
         <v>23</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="30">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="30"/>
       <c r="G8" s="31"/>
@@ -3852,16 +3855,16 @@
         <v>24</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="30">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="31"/>
@@ -3873,16 +3876,16 @@
         <v>25</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="30">
         <v>10</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" s="30"/>
       <c r="G10" s="31"/>
@@ -3894,16 +3897,16 @@
         <v>26</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="30">
         <v>15</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="31"/>
@@ -3915,16 +3918,16 @@
         <v>27</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="30">
         <v>20</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" s="30"/>
       <c r="G12" s="31"/>
@@ -3936,16 +3939,16 @@
         <v>28</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="30">
         <v>5</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F13" s="30"/>
       <c r="G13" s="31"/>
@@ -3957,16 +3960,16 @@
         <v>29</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" s="30">
         <v>10</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F14" s="30"/>
       <c r="G14" s="31"/>
@@ -3978,16 +3981,16 @@
         <v>30</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="30">
         <v>15</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15" s="30"/>
       <c r="G15" s="31"/>
@@ -3999,16 +4002,16 @@
         <v>31</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" s="30">
         <v>25</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F16" s="30"/>
       <c r="G16" s="31"/>
@@ -4020,16 +4023,16 @@
         <v>32</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="30">
         <v>10</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="31"/>
@@ -4041,16 +4044,16 @@
         <v>33</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="8">
         <v>30</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F18" s="30"/>
       <c r="G18" s="31"/>
@@ -4062,16 +4065,16 @@
         <v>34</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" s="30">
         <v>30</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="31"/>
@@ -4083,16 +4086,16 @@
         <v>35</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" s="30">
         <v>0</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F20" s="30"/>
       <c r="G20" s="31"/>
@@ -4104,16 +4107,16 @@
         <v>36</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D21" s="30">
         <v>20</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F21" s="30"/>
       <c r="G21" s="31"/>
@@ -4125,16 +4128,16 @@
         <v>37</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="30">
         <v>0</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F22" s="30"/>
       <c r="G22" s="31"/>
@@ -4146,16 +4149,16 @@
         <v>38</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D23" s="30">
         <v>10</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="31"/>
@@ -4167,16 +4170,16 @@
         <v>39</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D24" s="30">
         <v>10</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F24" s="30"/>
       <c r="G24" s="31"/>
@@ -4188,22 +4191,22 @@
         <v>40</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" s="30">
         <v>20</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F25" s="30"/>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
       <c r="I25" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -4211,22 +4214,22 @@
         <v>41</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D26" s="30">
         <v>20</v>
       </c>
       <c r="E26" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F26" s="30"/>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
       <c r="I26" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -4234,39 +4237,39 @@
         <v>42</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" s="30">
         <v>30</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
       <c r="I27" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D28" s="30">
         <v>10</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="31"/>
@@ -4275,19 +4278,19 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D29" s="30">
         <v>10</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="31"/>
@@ -4296,19 +4299,19 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="30" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D30" s="30">
         <v>60</v>
       </c>
       <c r="E30" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F30" s="30"/>
       <c r="G30" s="31"/>
@@ -4317,19 +4320,19 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="30" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B31" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="C31" s="30" t="s">
         <v>286</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>288</v>
       </c>
       <c r="D31" s="30">
         <v>0</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F31" s="30"/>
       <c r="G31" s="31"/>
@@ -4338,19 +4341,19 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D32" s="30">
         <v>10</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="31"/>
@@ -4359,19 +4362,19 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D33" s="30">
         <v>10</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F33" s="30"/>
       <c r="G33" s="31"/>
@@ -4380,19 +4383,19 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D34" s="30">
         <v>5</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F34" s="30"/>
       <c r="G34" s="31"/>
@@ -4401,19 +4404,19 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="30" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D35" s="30">
         <v>10</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F35" s="30"/>
       <c r="G35" s="31"/>
@@ -4422,19 +4425,19 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="30" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D36" s="30">
         <v>10</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F36" s="30"/>
       <c r="G36" s="31"/>
@@ -4443,19 +4446,19 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="30" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D37" s="30">
         <v>10</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F37" s="30"/>
       <c r="G37" s="31"/>
@@ -4464,19 +4467,19 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="30" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D38" s="30">
         <v>0</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F38" s="30"/>
       <c r="G38" s="31"/>
@@ -4485,19 +4488,19 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="30" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D39" s="30">
         <v>0</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F39" s="30"/>
       <c r="G39" s="31"/>
@@ -4506,19 +4509,19 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="30" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D40" s="30">
         <v>0</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F40" s="30"/>
       <c r="G40" s="31"/>
@@ -4527,19 +4530,19 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="30" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D41" s="30">
         <v>10</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F41" s="30"/>
       <c r="G41" s="31"/>
@@ -4548,19 +4551,19 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="30" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D42" s="30">
         <v>10</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F42" s="30"/>
       <c r="G42" s="31"/>
@@ -19945,22 +19948,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="59.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="95.140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="95.140625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
@@ -19970,819 +19972,744 @@
       <c r="C1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B2" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30">
+      <c r="A3" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>344</v>
+      </c>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:4" ht="30">
+      <c r="A4" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>345</v>
+      </c>
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="C5" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>331</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="33" t="s">
-        <v>346</v>
-      </c>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>331</v>
-      </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33" t="s">
-        <v>347</v>
-      </c>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>331</v>
-      </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="32" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>331</v>
-      </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>329</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="14"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="B12" s="33" t="s">
-        <v>328</v>
-      </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="32" t="s">
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="33" t="s">
-        <v>328</v>
-      </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="34" t="s">
+      <c r="B14" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="C14" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="B14" s="33" t="s">
-        <v>328</v>
-      </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="35" t="s">
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="34" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="34" t="s">
+      <c r="B15" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="C15" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="B15" s="33" t="s">
-        <v>328</v>
-      </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34" t="s">
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="C16" s="33" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>328</v>
-      </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>249</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
         <v>251</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="17" t="s">
+      <c r="B19" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30">
+      <c r="A21" t="s">
         <v>252</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>253</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="B21" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="7" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="16" t="s">
+      <c r="B22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30">
-      <c r="A21" t="s">
-        <v>254</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="17" t="s">
+    <row r="23" spans="1:3" ht="30">
+      <c r="A23" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="14" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30">
-      <c r="A23" s="8" t="s">
+    <row r="24" spans="1:3">
+      <c r="A24" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30">
+      <c r="A25" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30">
+      <c r="A31" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30">
+      <c r="A33" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30">
+      <c r="A34" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30">
+      <c r="A37" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30">
+      <c r="A41" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="30">
+      <c r="A44" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30">
+      <c r="A45" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30">
+      <c r="A50" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="30">
+      <c r="A52" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="30">
+      <c r="A54" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="30">
+      <c r="A55" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="30">
+      <c r="A57" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="30">
+      <c r="A58" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="30">
+      <c r="A62" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30">
+      <c r="A63" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="30">
+      <c r="A64" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="30">
+      <c r="A65" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="30">
+      <c r="A66" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="B67" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67" s="38"/>
+    </row>
+    <row r="68" spans="1:3" ht="30">
+      <c r="A68" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="14" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30">
-      <c r="A25" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="14" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="16" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="16" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="16" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="16" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30">
-      <c r="A31" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="16" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="16" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30">
-      <c r="A33" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="14" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30">
-      <c r="A34" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="14" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="16" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="16" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="30">
-      <c r="A37" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="16" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="14" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30">
-      <c r="A41" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="14" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="16" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30">
-      <c r="A44" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30">
-      <c r="A45" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="14" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="14" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="14" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="14" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="30">
-      <c r="A50" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="30">
-      <c r="A52" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="14" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="14" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="30">
-      <c r="A54" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="30">
-      <c r="A55" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="30">
-      <c r="A57" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="30">
-      <c r="A58" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C58" s="7"/>
-      <c r="D58" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" s="7"/>
-      <c r="D61" s="16" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="30">
-      <c r="A62" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="14" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="30">
-      <c r="A63" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="30">
-      <c r="A64" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B64" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C64" s="7"/>
-      <c r="D64" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="30">
-      <c r="A65" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C65" s="8"/>
-      <c r="D65" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="30">
-      <c r="A66" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C66" s="7"/>
-      <c r="D66" s="16" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="8" t="s">
+      <c r="B68" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" s="39" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="B67" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="14"/>
-      <c r="E67" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="30">
-      <c r="A68" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C68" s="7"/>
-      <c r="D68" s="16" t="s">
-        <v>348</v>
-      </c>
-      <c r="E68" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="14"/>
-      <c r="E69" t="s">
-        <v>237</v>
-      </c>
+      <c r="B69" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C69" s="38"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D44">
+  <autoFilter ref="A1:C44">
     <sortState ref="A2:D149">
       <sortCondition ref="A2:A149"/>
     </sortState>
@@ -20790,7 +20717,7 @@
   <conditionalFormatting sqref="A22:A26 A20 A1 A31:A1048576 A5 A7:A16">
     <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
+  <conditionalFormatting sqref="C15">
     <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
@@ -20820,7 +20747,7 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -20836,24 +20763,24 @@
         <v>4</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="90">
       <c r="A2" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>349</v>
+        <v>385</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>9</v>
@@ -20861,13 +20788,13 @@
     </row>
     <row r="3" spans="1:4" ht="210">
       <c r="A3" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>9</v>
@@ -21363,18 +21290,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60">
       <c r="A2" s="7" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>9</v>
@@ -21382,10 +21309,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>9</v>
@@ -21393,10 +21320,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>9</v>
@@ -21404,10 +21331,10 @@
     </row>
     <row r="5" spans="1:3" ht="29.25" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>9</v>
@@ -21415,10 +21342,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="7" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>9</v>
@@ -21426,10 +21353,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="7" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>9</v>
@@ -21437,10 +21364,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="7" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>9</v>
@@ -21448,10 +21375,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="7" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>9</v>
@@ -21459,10 +21386,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="7" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>9</v>
@@ -21470,10 +21397,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="7" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>9</v>
@@ -21481,10 +21408,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="7" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>9</v>
@@ -21492,10 +21419,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="7" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>9</v>
@@ -21503,10 +21430,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="7" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>9</v>
@@ -21514,10 +21441,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="7" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
@@ -21561,7 +21488,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>12</v>
@@ -21570,49 +21497,49 @@
         <v>14</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="25.5">
       <c r="A3" s="15" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="38.25">
       <c r="A4" s="18" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="28" t="s">
         <v>145</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>

<commit_message>
profile still not building from data.json
</commit_message>
<xml_diff>
--- a/data/hh3_data.xlsx
+++ b/data/hh3_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-3345" yWindow="10695" windowWidth="25815" windowHeight="15495" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-3345" yWindow="10695" windowWidth="25815" windowHeight="15495" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">options!$A$1:$I$1387</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">warning_rules!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1739,7 +1739,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1786,7 +1786,7 @@
         <xdr:cNvPr id="3" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1833,7 +1833,7 @@
         <xdr:cNvPr id="4" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2179,7 +2179,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2189,9 +2189,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -3559,8 +3559,8 @@
         <v>400</v>
       </c>
       <c r="H50" s="7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -19950,9 +19950,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -21473,8 +21473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C46" sqref="C42:D46"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
further fixing unit types
</commit_message>
<xml_diff>
--- a/data/hh3_data.xlsx
+++ b/data/hh3_data.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="426">
   <si>
     <t>model_id</t>
   </si>
@@ -1370,6 +1370,36 @@
   </si>
   <si>
     <t>sub-type</t>
+  </si>
+  <si>
+    <t>Apex Detachment Combat Retinue</t>
+  </si>
+  <si>
+    <t>Apex Detachment Officer Cadre</t>
+  </si>
+  <si>
+    <t>Apex Detachment Army Vanguard</t>
+  </si>
+  <si>
+    <t>Auxillary Detachment Armoured Fist</t>
+  </si>
+  <si>
+    <t>Auxillary Detachment Tactical Support</t>
+  </si>
+  <si>
+    <t>Auxillary Detachment Armoured Support</t>
+  </si>
+  <si>
+    <t>Auxillary Detachment Heavy Support</t>
+  </si>
+  <si>
+    <t>Auxillary Detachment Combat Pioneers</t>
+  </si>
+  <si>
+    <t>Auxillary Detachment Shock Assault</t>
+  </si>
+  <si>
+    <t>Auxillary Detachment First Strike</t>
   </si>
 </sst>
 </file>
@@ -1895,7 +1925,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1942,7 +1972,7 @@
         <xdr:cNvPr id="3" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1989,7 +2019,7 @@
         <xdr:cNvPr id="4" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2335,7 +2365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2346,8 +2376,8 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -2440,7 +2470,7 @@
         <v>292</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>292</v>
+        <v>416</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -2467,7 +2497,7 @@
         <v>294</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>294</v>
+        <v>417</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -2494,7 +2524,7 @@
         <v>293</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>293</v>
+        <v>418</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -2521,7 +2551,7 @@
         <v>295</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>295</v>
+        <v>419</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -2548,7 +2578,7 @@
         <v>296</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>296</v>
+        <v>420</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -2575,7 +2605,7 @@
         <v>297</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>297</v>
+        <v>421</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -2602,7 +2632,7 @@
         <v>298</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>298</v>
+        <v>422</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -2629,7 +2659,7 @@
         <v>299</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>299</v>
+        <v>423</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -2656,7 +2686,7 @@
         <v>300</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>300</v>
+        <v>424</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -2683,7 +2713,7 @@
         <v>301</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>301</v>
+        <v>425</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -3839,7 +3869,7 @@
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -20133,7 +20163,7 @@
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -21050,7 +21080,7 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -21578,7 +21608,7 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -21777,7 +21807,7 @@
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
fixing some special rules
</commit_message>
<xml_diff>
--- a/data/hh3_data.xlsx
+++ b/data/hh3_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-3345" yWindow="10695" windowWidth="25815" windowHeight="15495" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-3345" yWindow="10695" windowWidth="25815" windowHeight="15495" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -843,9 +843,6 @@
     <t>Attacks made with the Blast (X) Special Rule use a Blast Marker to determine how many Hits are caused.</t>
   </si>
   <si>
-    <t>With a Weapon that has the Breaching (X) Special Rule there is a chance that a Wound Test may result I nthe Wound ignoring Armour Saves.</t>
-  </si>
-  <si>
     <t>[astartes] legion-saturnine-praetor</t>
   </si>
   <si>
@@ -1057,9 +1054,6 @@
   </si>
   <si>
     <t>First Strike</t>
-  </si>
-  <si>
-    <t>May select a Rite of War. May select one Apex Detachment.</t>
   </si>
   <si>
     <t>Infantry</t>
@@ -1400,6 +1394,12 @@
   </si>
   <si>
     <t>Auxillary Detachment First Strike</t>
+  </si>
+  <si>
+    <t>I think this gives an Apex detachment.</t>
+  </si>
+  <si>
+    <t>With a Weapon that has the Breaching (X) Special Rule there is a chance that a Wound Test may result in the Wound ignoring Armour Saves.</t>
   </si>
 </sst>
 </file>
@@ -1925,7 +1925,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1972,7 +1972,7 @@
         <xdr:cNvPr id="3" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2019,7 +2019,7 @@
         <xdr:cNvPr id="4" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2365,7 +2365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2424,7 +2424,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>94</v>
@@ -2436,10 +2436,10 @@
         <v>63</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
@@ -2455,7 +2455,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>94</v>
@@ -2467,10 +2467,10 @@
         <v>63</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -2482,7 +2482,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>94</v>
@@ -2494,10 +2494,10 @@
         <v>63</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -2509,7 +2509,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>94</v>
@@ -2521,10 +2521,10 @@
         <v>63</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>94</v>
@@ -2548,10 +2548,10 @@
         <v>63</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>94</v>
@@ -2575,10 +2575,10 @@
         <v>63</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>94</v>
@@ -2602,10 +2602,10 @@
         <v>63</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>94</v>
@@ -2629,10 +2629,10 @@
         <v>63</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -2644,7 +2644,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>94</v>
@@ -2656,10 +2656,10 @@
         <v>63</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>94</v>
@@ -2683,10 +2683,10 @@
         <v>63</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -2698,7 +2698,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>94</v>
@@ -2710,10 +2710,10 @@
         <v>63</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -2725,7 +2725,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>94</v>
@@ -2737,10 +2737,10 @@
         <v>63</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -2752,7 +2752,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>94</v>
@@ -2764,10 +2764,10 @@
         <v>63</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>94</v>
@@ -2791,10 +2791,10 @@
         <v>63</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -2818,7 +2818,7 @@
         <v>63</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>55</v>
@@ -2833,7 +2833,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>94</v>
@@ -2845,7 +2845,7 @@
         <v>63</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>55</v>
@@ -2872,7 +2872,7 @@
         <v>63</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>55</v>
@@ -2899,7 +2899,7 @@
         <v>63</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>55</v>
@@ -2926,7 +2926,7 @@
         <v>63</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>56</v>
@@ -2953,7 +2953,7 @@
         <v>63</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>56</v>
@@ -2980,7 +2980,7 @@
         <v>63</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>56</v>
@@ -3007,7 +3007,7 @@
         <v>63</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>57</v>
@@ -3034,7 +3034,7 @@
         <v>63</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>57</v>
@@ -3061,7 +3061,7 @@
         <v>63</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>57</v>
@@ -3088,7 +3088,7 @@
         <v>63</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>56</v>
@@ -3115,10 +3115,10 @@
         <v>63</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G27" s="1">
         <v>115</v>
@@ -3142,10 +3142,10 @@
         <v>63</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G28" s="1">
         <v>115</v>
@@ -3157,7 +3157,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>94</v>
@@ -3169,7 +3169,7 @@
         <v>63</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>58</v>
@@ -3196,7 +3196,7 @@
         <v>63</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>58</v>
@@ -3223,7 +3223,7 @@
         <v>63</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>58</v>
@@ -3250,10 +3250,10 @@
         <v>63</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G32" s="1">
         <v>130</v>
@@ -3277,10 +3277,10 @@
         <v>63</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G33" s="1">
         <v>105</v>
@@ -3304,7 +3304,7 @@
         <v>63</v>
       </c>
       <c r="E34" s="34" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>59</v>
@@ -3331,7 +3331,7 @@
         <v>63</v>
       </c>
       <c r="E35" s="34" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F35" t="s">
         <v>59</v>
@@ -3358,7 +3358,7 @@
         <v>63</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F36" t="s">
         <v>127</v>
@@ -3385,7 +3385,7 @@
         <v>63</v>
       </c>
       <c r="E37" s="34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>59</v>
@@ -3412,7 +3412,7 @@
         <v>63</v>
       </c>
       <c r="E38" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>60</v>
@@ -3439,7 +3439,7 @@
         <v>63</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>60</v>
@@ -3466,7 +3466,7 @@
         <v>63</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>60</v>
@@ -3493,7 +3493,7 @@
         <v>63</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>60</v>
@@ -3520,7 +3520,7 @@
         <v>63</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>59</v>
@@ -3547,7 +3547,7 @@
         <v>63</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>61</v>
@@ -3574,7 +3574,7 @@
         <v>63</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>61</v>
@@ -3601,7 +3601,7 @@
         <v>63</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>62</v>
@@ -3628,7 +3628,7 @@
         <v>63</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>62</v>
@@ -3655,7 +3655,7 @@
         <v>63</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>62</v>
@@ -3682,7 +3682,7 @@
         <v>63</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>62</v>
@@ -3709,7 +3709,7 @@
         <v>63</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>151</v>
@@ -3751,7 +3751,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>94</v>
@@ -3763,10 +3763,10 @@
         <v>63</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G51" s="1">
         <v>80</v>
@@ -3778,7 +3778,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>94</v>
@@ -3790,10 +3790,10 @@
         <v>63</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G52" s="1">
         <v>75</v>
@@ -3805,7 +3805,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>94</v>
@@ -3817,7 +3817,7 @@
         <v>63</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>127</v>
@@ -3831,19 +3831,19 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>412</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>414</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>60</v>
@@ -3866,7 +3866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ1577"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
@@ -4322,7 +4322,7 @@
         <v>96</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D21" s="30">
         <v>20</v>
@@ -4469,13 +4469,13 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D28" s="30">
         <v>10</v>
@@ -4490,13 +4490,13 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D29" s="30">
         <v>10</v>
@@ -4511,13 +4511,13 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D30" s="30">
         <v>60</v>
@@ -4532,13 +4532,13 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D31" s="30">
         <v>0</v>
@@ -4553,13 +4553,13 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D32" s="30">
         <v>10</v>
@@ -4574,13 +4574,13 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D33" s="30">
         <v>10</v>
@@ -4595,13 +4595,13 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D34" s="30">
         <v>5</v>
@@ -4616,13 +4616,13 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="30" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D35" s="30">
         <v>10</v>
@@ -4637,13 +4637,13 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="30" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D36" s="30">
         <v>10</v>
@@ -4658,13 +4658,13 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="30" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D37" s="30">
         <v>10</v>
@@ -4679,13 +4679,13 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="30" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D38" s="30">
         <v>0</v>
@@ -4700,13 +4700,13 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="30" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D39" s="30">
         <v>0</v>
@@ -4721,13 +4721,13 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="30" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D40" s="30">
         <v>0</v>
@@ -4742,13 +4742,13 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="30" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D41" s="30">
         <v>10</v>
@@ -4763,13 +4763,13 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="30" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D42" s="30">
         <v>10</v>
@@ -20162,9 +20162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -20190,10 +20190,10 @@
         <v>160</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">
@@ -20201,10 +20201,10 @@
         <v>159</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D3" s="14"/>
     </row>
@@ -20213,10 +20213,10 @@
         <v>93</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D4" s="14"/>
     </row>
@@ -20225,87 +20225,87 @@
         <v>92</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>331</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="32" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45">
       <c r="A7" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="60">
       <c r="A8" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="105">
       <c r="A9" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="120">
       <c r="A10" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75">
       <c r="A11" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45">
       <c r="A12" s="8" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="60">
@@ -20313,98 +20313,98 @@
         <v>56</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30">
       <c r="A16" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="90">
       <c r="A17" s="8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="75">
       <c r="A18" s="8" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30">
       <c r="A19" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45">
       <c r="A20" s="8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="105">
       <c r="A21" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -20412,7 +20412,7 @@
         <v>129</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C22" s="33" t="s">
         <v>131</v>
@@ -20423,7 +20423,7 @@
         <v>132</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C23" s="35" t="s">
         <v>130</v>
@@ -20434,7 +20434,7 @@
         <v>133</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C24" s="35" t="s">
         <v>134</v>
@@ -20445,7 +20445,7 @@
         <v>135</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C25" s="34" t="s">
         <v>136</v>
@@ -20456,7 +20456,7 @@
         <v>138</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C26" s="33" t="s">
         <v>137</v>
@@ -20536,7 +20536,7 @@
         <v>44</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>259</v>
+        <v>425</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -21029,7 +21029,7 @@
         <v>44</v>
       </c>
       <c r="C78" s="39" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -21113,7 +21113,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>9</v>
@@ -21631,10 +21631,10 @@
     </row>
     <row r="2" spans="1:3" ht="60">
       <c r="A2" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>9</v>
@@ -21642,7 +21642,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>153</v>
@@ -21653,7 +21653,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>140</v>
@@ -21664,7 +21664,7 @@
     </row>
     <row r="5" spans="1:3" ht="29.25" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>128</v>
@@ -21675,10 +21675,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>9</v>
@@ -21686,7 +21686,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>142</v>
@@ -21697,10 +21697,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>9</v>
@@ -21708,10 +21708,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>9</v>
@@ -21719,7 +21719,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>141</v>
@@ -21730,10 +21730,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>9</v>
@@ -21741,10 +21741,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>9</v>
@@ -21752,10 +21752,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>9</v>
@@ -21763,10 +21763,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>9</v>
@@ -21774,7 +21774,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>140</v>
@@ -21849,13 +21849,13 @@
     </row>
     <row r="3" spans="1:4" ht="25.5">
       <c r="A3" s="15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>154</v>
@@ -21863,7 +21863,7 @@
     </row>
     <row r="4" spans="1:4" ht="38.25">
       <c r="A4" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
updated Vite and minor files
</commit_message>
<xml_diff>
--- a/data/hh3_data.xlsx
+++ b/data/hh3_data.xlsx
@@ -3322,7 +3322,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3369,7 +3369,7 @@
         <xdr:cNvPr id="3" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3416,7 +3416,7 @@
         <xdr:cNvPr id="4" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3762,7 +3762,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3773,8 +3773,8 @@
   <dimension ref="A1:L224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -6556,7 +6556,7 @@
         <v>376</v>
       </c>
       <c r="G77" s="1">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H77" s="1">
         <v>10</v>
@@ -6631,7 +6631,7 @@
         <v>18</v>
       </c>
       <c r="H79" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I79" s="1">
         <v>5</v>

</xml_diff>